<commit_message>
Squishes neighboring text runs into one if compatible.
git-svn-id: https://okapi.googlecode.com/svn/trunk@1973 0cd2bb99-014b-0410-b875-5d0485b745ed
</commit_message>
<xml_diff>
--- a/filters/net.sf.okapi.filters.openxml.tests/data/sampleMore.xlsx
+++ b/filters/net.sf.okapi.filters.openxml.tests/data/sampleMore.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="20055" windowHeight="12240"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="19320" windowHeight="12120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,6 @@
     <t>ipsum</t>
   </si>
   <si>
-    <t>dolor</t>
-  </si>
-  <si>
     <t>sit</t>
   </si>
   <si>
@@ -46,13 +43,28 @@
   </si>
   <si>
     <t>at</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">dolor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>osa</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +112,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -444,7 +463,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -470,7 +489,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>333</v>
@@ -478,7 +497,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>444</v>
@@ -486,7 +505,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>555</v>
@@ -494,7 +513,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>666</v>
@@ -502,7 +521,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>777</v>
@@ -510,7 +529,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>888</v>
@@ -518,7 +537,7 @@
     </row>
     <row r="9" spans="1:2" ht="30">
       <c r="A9" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>999</v>
@@ -526,7 +545,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <f>SUM(B1:B9)</f>

</xml_diff>